<commit_message>
Adding late Abstract entry 127
</commit_message>
<xml_diff>
--- a/AssetsHonsPrelimTA2024/data/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
+++ b/AssetsHonsPrelimTA2024/data/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherbean/Documents/GitHub/drcgb.github.io/AssetsHonsPrelimTA2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF6CFCC-82AC-FD4E-98F6-56BAA749DE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F32A20E-B72E-C94A-B67B-1D44C3C83534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26880" xr2:uid="{D65AE397-B8D4-2049-9FF4-B8C90A09C2A0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="301">
   <si>
     <t>Abstract ID</t>
   </si>
@@ -1016,6 +1016,12 @@
   </si>
   <si>
     <t>Background: Family medicine/general practice (FM/GP) trainees are increasingly recognised as at risk of occupational burnout, highlighting a need to examine which interventions are effective. Aims: To systematically review and quantitatively assess the empirical evidence for psychosocial interventions targeted to FM/GP trainees to reduce burnout and/or promote well-being. Methods: Eligible studies included FM/GP trainees undergoing psychosocial interventions aimed at reducing burnout/improving well-being. A large search on databases such as PsycInfo, Medline, Embase and ProQuest was performed without date restrictions. Studies were assessed by two reviewers for their risk of bias, using the Mixed Methods Appraisal Tool (MMAT) and achieved high inter-rater agreement (88%). Hedges' g effect size estimations were used to synthesise the data and pooled across trials using a random effects model. Publication bias was evaluated and causes of heterogeneity were investigated using moderator analyses. Results: Thirteen studies including 230 FM/GP trainees were included, with interventions focusing on organisational and individual levels. Individually based interventions showed a moderately large and statistically significant treatment effect (g = 0.483, 95% CI [0.096, 0.870], p &lt;.05), however group differences were not observed. Qualitative feedback received from participants suggested interventions should focus on the importance of curriculum modifications and organised group support. Conclusions: Although some results displayed statistical significance, these results should be regarded cautiously because of the small sample sizes and possible bias. Overall, the findings of this study highlight the severity of burnout and its effects on well-being and the need for interventions to reduce these symptoms. Protocol was registered on Open Science Framework (osf.io/xxxx). Keywords: Burnout, Family Medicine, General Practice, Trainee</t>
+  </si>
+  <si>
+    <t>Investigating attitudes towards AI and its impact on the relationships between work stress and emotional eating.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In recent literature, the intricate interplay between workplace stress and emotional eating has garnered significant attention. This dynamic relationship reflects the multifaceted nature of human behaviour within organisational settings. Research indicates that heightened levels of stress in the workplace often trigger maladaptive coping mechanisms, with emotional eating emerging as a prevalent response. Individuals may turn to food as a means of seeking comfort or alleviating negative emotions induced by work-related pressures. Exploring the connection between workplace stress and attitudes toward Artificial Intelligence (AI) in organisational settings poses an opportunity to look at the intersection of human psychology, technological advancement, and organisational dynamics. As AI increasingly pervades various aspects of work, from automation to decision support systems, its integration often elicits a spectrum of reactions among employees, ranging from enthusiasm to apprehension. Delving into the complex relationship among workplace stress, attitudes toward Artificial Intelligence (AI) in the workplace, and its impact on emotional eating will offer a comprehensive understanding of the modern organisational landscape. In this study, participants were recruited from diverse demographics to ensure representative sample. Participants completed the self-reported questionnaire assessing their perceived stress levels in the workplace, feelings of burnout, attitudes towards AI, and frequency of emotional eating behaviours. </t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1945,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BFD390-3B9D-B84B-A0C7-E2BE4A98CFC4}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K120"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="DP121" sqref="DP121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5282,6 +5288,29 @@
       <c r="J120" s="11"/>
       <c r="K120" s="11"/>
     </row>
+    <row r="121" spans="1:11" ht="255" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>127</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>